<commit_message>
refactoring: just about to remove functionality from calendarViewCtrl to CalendarSelectStrategy.js
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -9,32 +9,59 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$9</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>Add default behavior for report cards</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
   <si>
-    <t>Create images for buttons</t>
-  </si>
-  <si>
-    <t>Implement "move event" functionality</t>
-  </si>
-  <si>
-    <t>Format the report fields (Start, End, Total) and their corresponding values</t>
-  </si>
-  <si>
-    <t>Implement the "today" button functionality or remove button</t>
-  </si>
-  <si>
-    <t>Replace native calendar buttons with app buttons</t>
+    <t>done</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>current</t>
+  </si>
+  <si>
+    <t>Report cards have default behavior</t>
+  </si>
+  <si>
+    <t>Buttons have images</t>
+  </si>
+  <si>
+    <t>Moving an event is reflected in the reports</t>
+  </si>
+  <si>
+    <t>Report fields are appealing</t>
+  </si>
+  <si>
+    <t>The 'today' button works correctly</t>
+  </si>
+  <si>
+    <t>Calendar navigation buttons match the card style</t>
+  </si>
+  <si>
+    <t>Refactor controller (architecture)</t>
+  </si>
+  <si>
+    <t>Report cards shows data for whole day, when calendar view is day</t>
   </si>
 </sst>
 </file>
@@ -376,53 +403,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="67.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C9">
+    <filterColumn colId="2">
+      <filters blank="1">
+        <filter val="pending"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Moved functionality to strategy
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
@@ -62,6 +62,15 @@
   </si>
   <si>
     <t>Report cards shows data for whole day, when calendar view is day</t>
+  </si>
+  <si>
+    <t>Deleting an event has the appropriate behavior if calendar is on day view</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Either the work day is 8 hours, or the 9 = 100% (fix the status bar)</t>
   </si>
 </sst>
 </file>
@@ -404,10 +413,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,10 +534,32 @@
         <v>2</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C9">
     <filterColumn colId="2">
-      <filters blank="1">
+      <filters>
         <filter val="pending"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Partially moved functionality to EventManager (delete, set current)
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
@@ -67,10 +67,16 @@
     <t>Deleting an event has the appropriate behavior if calendar is on day view</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Either the work day is 8 hours, or the 9 = 100% (fix the status bar)</t>
+  </si>
+  <si>
+    <t>high</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>When event is deleted the stats card behaves correctly</t>
   </si>
 </sst>
 </file>
@@ -413,10 +419,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +542,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
@@ -547,12 +553,23 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moving functionality ... something broke :(
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>When event is deleted the stats card behaves correctly</t>
+  </si>
+  <si>
+    <t>When no event is selected (stats in default mode) and an event is edied in day-view, the stats card behaves correctly</t>
   </si>
 </sst>
 </file>
@@ -419,15 +422,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="67.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -570,6 +573,17 @@
         <v>19</v>
       </c>
       <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modifying an event in the calendar (drag, stretch, etc) updates the stats card.
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$9</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$14</definedName>
   </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>current</t>
   </si>
   <si>
     <t>Report cards have default behavior</t>
@@ -425,7 +422,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +446,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -471,7 +468,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
@@ -482,7 +479,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -493,7 +490,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>2</v>
@@ -504,7 +501,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
         <v>2</v>
@@ -515,21 +512,21 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -537,7 +534,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>2</v>
@@ -545,50 +542,50 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
       <c r="C12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
         <v>19</v>
       </c>
-      <c r="C13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C9">
+  <autoFilter ref="A1:C14">
     <filterColumn colId="2">
       <filters>
         <filter val="pending"/>

</xml_diff>

<commit_message>
Added scaffolding for calendar directive
</commit_message>
<xml_diff>
--- a/bl.xlsx
+++ b/bl.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Refactor css classes for link cards</t>
   </si>
@@ -77,6 +77,12 @@
   </si>
   <si>
     <t>When no event is selected (stats in default mode) and an event is edied in day-view, the stats card behaves correctly</t>
+  </si>
+  <si>
+    <t>Day meter card contains day stats</t>
+  </si>
+  <si>
+    <t>Calendar is wrapped in a directive</t>
   </si>
 </sst>
 </file>
@@ -419,10 +425,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +588,22 @@
       </c>
       <c r="C14" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>